<commit_message>
Chain production done with only not-none df
- Takes too long (Even with 20 entries)
- How to optimize(?)
- Implement None columns
</commit_message>
<xml_diff>
--- a/venv/Degistirilmis.xlsx
+++ b/venv/Degistirilmis.xlsx
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
         <v>182</v>
@@ -544,14 +544,14 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>İZMİR</t>
+          <t>DİYARBAKIR</t>
         </is>
       </c>
       <c r="G3" t="n">
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>195</v>
@@ -584,7 +584,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>DİYARBAKIR</t>
+          <t>KARABÜK</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -624,7 +624,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>İSTANBUL</t>
+          <t>GİRESUN</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -664,14 +664,14 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>GİRESUN</t>
+          <t>İZMİR</t>
         </is>
       </c>
       <c r="G6" t="n">
         <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
         <v>176</v>
@@ -704,14 +704,14 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>DİYARBAKIR</t>
+          <t>GİRESUN</t>
         </is>
       </c>
       <c r="G7" t="n">
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7" t="n">
         <v>182</v>
@@ -744,14 +744,14 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>GİRESUN</t>
+          <t>KARABÜK</t>
         </is>
       </c>
       <c r="G8" t="n">
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>195</v>
@@ -784,7 +784,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>KARABÜK</t>
+          <t>DİYARBAKIR</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>KARABÜK</t>
+          <t>İSTANBUL</t>
         </is>
       </c>
       <c r="G11" t="n">

</xml_diff>